<commit_message>
Script executes from start to finish on Bacillus tree
Script executes on Bacillus Tree
</commit_message>
<xml_diff>
--- a/excel_files/Comparison - AP011541 & Ancestor 10.xlsx
+++ b/excel_files/Comparison - AP011541 & Ancestor 10.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="71">
   <si>
     <t>AP011541</t>
   </si>
@@ -77,118 +77,154 @@
     <t>-[Phe_UUC, Asp_GAC, Glu_GAA, Lys_AAA]</t>
   </si>
   <si>
+    <t>[ , S,e,r,_,U,C,A]</t>
+  </si>
+  <si>
+    <t>[16S, Ile_AUC,Ala_GCA,23S,5S]</t>
+  </si>
+  <si>
     <t>[Met_AUG, Glu_GAA]</t>
   </si>
   <si>
-    <t>[Glu_GAA, Val_GUA, Thr_ACA, Tyr_UAC, Gln_CAA]</t>
-  </si>
-  <si>
-    <t>[16S, 23S, 5S, 16S, 23S, 5S]</t>
+    <t>[16S, 23S,5S,Asn_AAC,Thr_ACC,Gly_GGC,Arg_CGU,Pro_CCA,Ala_GCA,16S,23S,5S,16S,23S,5S]</t>
+  </si>
+  <si>
+    <t>[Glu_GAA, Val_GUA,Thr_ACA,Tyr_UAC,Gln_CAA]</t>
+  </si>
+  <si>
+    <t>[Arg_CGU, Gly_GGA,16S,23S,5S,Met_AUG,Asp_GAC]</t>
+  </si>
+  <si>
+    <t>[16S, 23S,5S,Asn_AAC,Ser_UCC,Glu_GAA,Val_GUA,Met_AUG,Asp_GAC,Phe_UUC,Thr_ACA,Tyr_UAC,Trp_UGG,His_CAC,Gln_CAA,Gly_GGC,Cys_UGC,Leu_UUA,Leu_UUG]</t>
+  </si>
+  <si>
+    <t>[ , G,l,y,_,G,G,A]</t>
+  </si>
+  <si>
+    <t>[ , V,a,l,_,G,U,C]</t>
+  </si>
+  <si>
+    <t>[ , -,A,r,g,_,A,G,G]</t>
+  </si>
+  <si>
+    <t>[ , G,l,n,_,C,A,A]</t>
+  </si>
+  <si>
+    <t>[ , -,A,r,g,_,A,G,A]</t>
+  </si>
+  <si>
+    <t>[ , -,A,l,a,_,G,C,C]</t>
+  </si>
+  <si>
+    <t>[ , -,A,r,g,_,C,G,G]</t>
+  </si>
+  <si>
+    <t>[Phe_UUC, Asp_GAC,Glu_GAA,Lys_AAA]</t>
+  </si>
+  <si>
+    <t>[Ile_AUC, Ala_GCA,23S,5S]</t>
+  </si>
+  <si>
+    <t>[Asn_AAC, Ser_AGC,Glu_GAA,Gln_CAA,Lys_AAA,Leu_CUA]</t>
+  </si>
+  <si>
+    <t>[Glu_GAA, Ser_AGC,Asn_AAC,Ile_AUC,Gly_GGA,His_CAC,Phe_UUC,Asp_GAC,Met_AUG,Ser_UCA,Met_AUG,Met_AUG,Ala_GCA,Pro_CCA,Arg_CGU,Leu_UUA,Gly_GGC,Leu_CUG,Lys_AAA,Thr_ACA,Val_GUA,5S,23S,Ala_GCA,Ile_AUC]</t>
+  </si>
+  <si>
+    <t>[[, 1,6,S,,, ,2,3,S,,, ,5,S,,, ,1,6,S,,, ,2,3,S,,, ,5,S,]]</t>
+  </si>
+  <si>
+    <t>[[, 1,6,S,,, ,2,3,S,,, ,5,S,,, ,V,a,l,_,G,U,A,,, ,T,h,r,_,A,C,A,,, ,L,y,s,_,A,A,A,,, ,L,e,u,_,C,U,A,,, ,G,l,y,_,G,G,C,,, ,L,e,u,_,U,U,A,,, ,A,r,g,_,C,G,U,,, ,P,r,o,_,C,C,A,,, ,A,l,a,_,G,C,A,,, ,1,6,S,,, ,2,3,S,,, ,5,S,]]</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>0.0*</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>1.0*</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>33.0</t>
+  </si>
+  <si>
+    <t>123.0</t>
   </si>
   <si>
     <t>-999</t>
   </si>
   <si>
-    <t>0.0*</t>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>23.0</t>
   </si>
   <si>
     <t>7.0</t>
   </si>
   <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>18.0</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>23.0</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>0*</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>20.5</t>
-  </si>
-  <si>
-    <t>8.5</t>
+    <t>16.0</t>
   </si>
   <si>
     <t>19.0</t>
   </si>
   <si>
-    <t>11.0</t>
-  </si>
-  <si>
-    <t>17.0</t>
-  </si>
-  <si>
-    <t>16.0</t>
-  </si>
-  <si>
-    <t>14.0</t>
+    <t>24.0</t>
   </si>
   <si>
     <t>16.5</t>
   </si>
   <si>
-    <t>15.5</t>
-  </si>
-  <si>
-    <t>18.5</t>
-  </si>
-  <si>
-    <t>22.5</t>
-  </si>
-  <si>
-    <t>23.5</t>
-  </si>
-  <si>
-    <t>13.0</t>
-  </si>
-  <si>
-    <t>21.5</t>
-  </si>
-  <si>
-    <t>15.0</t>
-  </si>
-  <si>
-    <t>26.0</t>
-  </si>
-  <si>
-    <t>25.0</t>
-  </si>
-  <si>
     <t>21.0</t>
   </si>
   <si>
-    <t>25.5</t>
-  </si>
-  <si>
-    <t>22.0</t>
-  </si>
-  <si>
-    <t>24.0</t>
+    <t>24.0*</t>
+  </si>
+  <si>
+    <t>4.0*</t>
   </si>
   <si>
     <t>4.0</t>
@@ -543,64 +579,64 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -608,129 +644,129 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="S3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="U3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="V3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
+      <c r="C4" t="s">
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -738,64 +774,64 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="S5" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="T5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="V5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -806,64 +842,64 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="T6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="U6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="V6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -871,64 +907,64 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="Q7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="R7" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="S7" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="T7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="U7" t="s">
-        <v>30</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
+      </c>
+      <c r="V7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -936,64 +972,64 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s">
         <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="R8" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="S8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="T8" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="U8" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="V8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1001,64 +1037,64 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9" t="s">
+        <v>61</v>
+      </c>
+      <c r="U9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="V9" t="s">
         <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>27</v>
-      </c>
-      <c r="R9" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" t="s">
-        <v>40</v>
-      </c>
-      <c r="T9" t="s">
-        <v>52</v>
-      </c>
-      <c r="U9" t="s">
-        <v>43</v>
-      </c>
-      <c r="V9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1066,64 +1102,64 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O10" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="T10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="U10" t="s">
         <v>49</v>
       </c>
       <c r="V10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1131,64 +1167,64 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
         <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11" t="s">
         <v>42</v>
       </c>
-      <c r="J11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" t="s">
-        <v>28</v>
-      </c>
       <c r="S11" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="T11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="U11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="V11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1196,64 +1232,64 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="L12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="O12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="P12" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="R12" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="T12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="U12" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="V12" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1261,64 +1297,64 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
       </c>
       <c r="K13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1326,64 +1362,64 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
+        <v>51</v>
       </c>
       <c r="L14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V14" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -1391,64 +1427,64 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="L15" t="s">
+        <v>51</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1456,64 +1492,64 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="M16" t="s">
+        <v>51</v>
       </c>
       <c r="N16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V16" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:22">
@@ -1521,64 +1557,64 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="N17" t="s">
+        <v>51</v>
       </c>
       <c r="O17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V17" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:22">
@@ -1586,64 +1622,64 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="N18" t="s">
+        <v>51</v>
       </c>
       <c r="O18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="P18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V18" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:22">
@@ -1651,64 +1687,64 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="s">
         <v>48</v>
       </c>
-      <c r="G19" t="s">
-        <v>53</v>
-      </c>
       <c r="H19" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="L19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="N19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="O19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="P19" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="Q19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="R19" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="S19" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="U19" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V19" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:22">
@@ -1716,64 +1752,64 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N20" t="s">
-        <v>23</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="O20" t="s">
+        <v>51</v>
       </c>
       <c r="P20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="Q20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:22">
@@ -1781,64 +1817,64 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="J21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="N21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="O21" t="s">
-        <v>23</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="P21" t="s">
+        <v>51</v>
       </c>
       <c r="Q21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="S21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="T21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="U21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="V21" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="2:22">
@@ -1846,64 +1882,64 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="H22" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="N22" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O22" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="R22" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="S22" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="T22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="U22" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="V22" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1926,64 +1962,64 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:22">

</xml_diff>